<commit_message>
add coment and prettify result
</commit_message>
<xml_diff>
--- a/goldendata_extracted_feature.xlsx
+++ b/goldendata_extracted_feature.xlsx
@@ -8,14 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github Repository\ta-newsX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAAE01E3-BDF0-4A79-A32E-4FE2D0ACBCB2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{213D773B-C42A-4BC0-B1C5-9FBB90ECE4E2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1600,7 +1607,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15172" uniqueCount="1486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7586" uniqueCount="1486">
   <si>
     <t>dist</t>
   </si>
@@ -6538,11 +6545,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2527"/>
+  <dimension ref="A1:H2529"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2516" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J2525" sqref="J2525"/>
+      <pane ySplit="1" topLeftCell="A2414" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F2529" sqref="F2529"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -72250,6 +72257,18 @@
       </c>
       <c r="H2527">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2528" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H2528">
+        <f>COUNTIF(H2:H2527,1)</f>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2529" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E2529">
+        <f>2*(57.8947*56.4103/(57.8947+56.4103))</f>
+        <v>57.142861561786447</v>
       </c>
     </row>
   </sheetData>

</xml_diff>